<commit_message>
ng: updated tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/ng_lf_tas_202402_2_participant_jgw.xlsx
+++ b/LF/TAS/Nigeria/2024/ng_lf_tas_202402_2_participant_jgw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB58082-336F-43D9-A61F-93997FC24E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CFCE37-32E9-41F1-BD75-775CE64D54B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -135,12 +135,6 @@
     <t>Enter age in years</t>
   </si>
   <si>
-    <t>. &gt;= 5 and . &lt;= 15</t>
-  </si>
-  <si>
-    <t>The age must be between 5 and 15 years</t>
-  </si>
-  <si>
     <t>p_how_long_lived</t>
   </si>
   <si>
@@ -240,35 +234,64 @@
     <t>school</t>
   </si>
   <si>
-    <t>p_index</t>
-  </si>
-  <si>
-    <t>Index in village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(${last-saved#p_index}!=null,${last-saved#p_index} + 1,1)
-</t>
-  </si>
-  <si>
     <t>Participant ID</t>
   </si>
   <si>
     <t>Write this code on the FTS stickers</t>
   </si>
   <si>
-    <t>concat(${p_recorder_id}, '-', ${p_cluster_id}, '-', ${p_index})</t>
-  </si>
-  <si>
     <t>regex(., '^.{0,255}$')</t>
   </si>
   <si>
     <t>The text is too long. It mys not exceed 255 caracters</t>
   </si>
   <si>
-    <t>ng_lf_tas_202402_2_participant_jgw_v1</t>
-  </si>
-  <si>
-    <t>(2024 Fev) Nigeria - 2. TAS1 LF Participants Form - Jigawa V1</t>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>begin repeat</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>position(..)</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>join(' ', ${p_code_id})</t>
+  </si>
+  <si>
+    <t>if (${C2} = 1,'',substring-after(${C1},${p_code_id}))</t>
+  </si>
+  <si>
+    <t>This barcode/QR Colde is already entered</t>
+  </si>
+  <si>
+    <t>not(selected(${C3}, ${p_code_id}))</t>
+  </si>
+  <si>
+    <t>end repeat</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>(2024 Fev) Nigeria - 2. TAS1 LF Participants Form - Jigawa V2.1</t>
+  </si>
+  <si>
+    <t>ng_lf_tas_202402_2_participant_jgw_v2_1</t>
+  </si>
+  <si>
+    <t>ng_p_202402_v2_1</t>
   </si>
 </sst>
 </file>
@@ -284,44 +307,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -339,16 +336,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor rgb="FFFBE4D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFBE4D5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -386,50 +434,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,365 +810,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="42.625" customWidth="1"/>
-    <col min="4" max="4" width="41.25" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="16.875" customWidth="1"/>
-    <col min="7" max="7" width="29.5" customWidth="1"/>
-    <col min="8" max="8" width="20.375" customWidth="1"/>
-    <col min="9" max="9" width="51.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.75" customWidth="1"/>
-    <col min="11" max="11" width="35.375" customWidth="1"/>
-    <col min="12" max="12" width="13.875" customWidth="1"/>
-    <col min="13" max="13" width="36.625" customWidth="1"/>
+    <col min="1" max="1" width="19.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="6" customWidth="1"/>
+    <col min="3" max="3" width="42.625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="41.25" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="29.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="20.375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="51.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="6" customWidth="1"/>
+    <col min="11" max="11" width="35.375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="36.625" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="37.5">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="37.5">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="47.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="47.25">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="3" customFormat="1">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:14" s="7" customFormat="1">
+      <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="D3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="15"/>
-    </row>
-    <row r="4" spans="1:14" s="3" customFormat="1">
-      <c r="A4" s="15" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" s="7" customFormat="1">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="D4" s="23"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="15"/>
-    </row>
-    <row r="5" spans="1:14" s="3" customFormat="1">
-      <c r="A5" s="15" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" s="7" customFormat="1">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="D5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" s="7" customFormat="1">
+      <c r="A6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" s="7" customFormat="1" ht="31.5">
+      <c r="A7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" s="7" customFormat="1">
+      <c r="A8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" s="7" customFormat="1">
+      <c r="A9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" s="7" customFormat="1">
+      <c r="A10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" s="3" customFormat="1">
-      <c r="A7" s="3" t="s">
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" s="7" customFormat="1">
+      <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B11" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C11" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="I11" s="23"/>
+      <c r="J11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" s="7" customFormat="1" ht="31.5">
+      <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="C13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="D13" s="23"/>
+      <c r="F13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
+      <c r="J13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" s="3" customFormat="1" ht="31.5">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="F9" s="3" t="s">
+    </row>
+    <row r="14" spans="1:14" s="7" customFormat="1">
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="C14" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="7" customFormat="1" ht="31.5">
+      <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="B15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="H15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" s="7" customFormat="1">
+      <c r="A16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="F16" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="G16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="3" customFormat="1">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="3" customFormat="1" ht="31.5">
-      <c r="A12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="H12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1">
-      <c r="A13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+    </row>
+    <row r="18" spans="1:13" s="7" customFormat="1">
+      <c r="A18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="B18" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="F13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="3" customFormat="1">
-      <c r="A14" s="3" t="s">
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1091,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1100,79 +1276,79 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+      <c r="C5" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1185,37 +1361,37 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="53.375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="34.75" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" style="14" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="14"/>
+    <col min="1" max="1" width="53.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="34.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>